<commit_message>
meta title changes to many pages (useeffect, other methods tried, etc. - it didn't work to hold the meta title - might have to undo this after some time (these chagnes))
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/360 melgroups creation 1/next db table stuff 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/360 melgroups creation 1/next db table stuff 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/360 melgroups creation 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864B8D14-18F3-784E-B310-BAC8EACB9F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE271131-C307-D142-85DA-FCA9525C052E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{A42B39F3-E3D9-AF44-A25F-37E3CC8EFA25}"/>
   </bookViews>
@@ -502,8 +502,8 @@
   <dimension ref="E1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>